<commit_message>
[Test] Update brio.xlsx test file
</commit_message>
<xml_diff>
--- a/tests/data/brio.xlsx
+++ b/tests/data/brio.xlsx
@@ -20,44 +20,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roumanie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belgique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+  <si>
+    <t xml:space="preserve">N° de BdL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tDate livraison réelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palettes sol 80*120 réellement reçues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palettes sol 100*120 réellement reçues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palettes EUR 80*120 réellement reçues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tStatut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tCommentaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/09/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annulée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 pal; annulee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">livrée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 pal; livree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/09/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x pal; annulee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/09/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COL050918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/09/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COL060918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas de date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COL170918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/05/1235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date avant 1900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/09/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orig doublon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83936990_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doublon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83936990_RET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -117,8 +188,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -139,15 +214,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -163,61 +245,241 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>3009454948</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>3009454949</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>3009690269</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>5</v>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
+        <v>3009819993</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>83936990</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>5</v>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Test] Change Bio.xlsx file to remove useless coma
</commit_message>
<xml_diff>
--- a/tests/data/brio.xlsx
+++ b/tests/data/brio.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t xml:space="preserve">N° de BdL</t>
   </si>
@@ -46,9 +46,6 @@
     <t xml:space="preserve">07/09/2018</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
     <t xml:space="preserve">annulée</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">21/09/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,</t>
   </si>
   <si>
     <t xml:space="preserve">x pal; annulee</t>
@@ -188,12 +182,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,18 +215,18 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -265,17 +263,17 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,17 +286,17 @@
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,22 +304,22 @@
         <v>3009690269</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,88 +327,88 @@
         <v>3009819993</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,27 +416,27 @@
         <v>83936990</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -446,22 +444,22 @@
       <c r="C10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>7</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -469,17 +467,17 @@
       <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>